<commit_message>
Implement bpixel, bformat, bpitch. Actually apply these to class 0x1C mthd 0300,0308,030c. Temporary ROP code too.
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/NV128.xlsx
+++ b/doc/nvidia_notes/NV128.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E099BA4-173F-4389-91B2-138C7153A05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48D7A92-8594-4E83-91A2-8770FEAA41A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1D03AB2B-52FC-42D1-A358-4DB83B150D6F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>RIVA128 to do:</t>
   </si>
@@ -130,6 +130,12 @@
       </rPr>
       <t>TODO: Research)</t>
     </r>
+  </si>
+  <si>
+    <t>300, 308, 30c done, rest not done</t>
+  </si>
+  <si>
+    <t>NONE</t>
   </si>
 </sst>
 </file>
@@ -164,12 +170,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -184,11 +202,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,169 +523,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7D5DA9-A0C6-4217-AFB0-C28D22984443}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
pull out the notifier object.
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/NV128.xlsx
+++ b/doc/nvidia_notes/NV128.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48D7A92-8594-4E83-91A2-8770FEAA41A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AAAD45-12B9-4C6E-9550-C5E2A1407CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1D03AB2B-52FC-42D1-A358-4DB83B150D6F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>RIVA128 to do:</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>NONE</t>
+  </si>
+  <si>
+    <t>Dumb Framebuffer (DFB)</t>
+  </si>
+  <si>
+    <t>Cursor (RAMDAC_CU)</t>
   </si>
 </sst>
 </file>
@@ -523,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7D5DA9-A0C6-4217-AFB0-C28D22984443}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -757,6 +763,16 @@
         <v>6</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rename name to param to represent that it is the parameter. Add pixel writing code, add rectangle rendering code. Implement ROP, Rectangle and Clip class methods. However, the drivers BSOD.
</commit_message>
<xml_diff>
--- a/doc/nvidia_notes/NV128.xlsx
+++ b/doc/nvidia_notes/NV128.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\86Box\doc\nvidia_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AAAD45-12B9-4C6E-9550-C5E2A1407CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C80209-57A4-488F-BD3B-F8F9FD0BBFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1D03AB2B-52FC-42D1-A358-4DB83B150D6F}"/>
+    <workbookView xWindow="11610" yWindow="1590" windowWidth="28800" windowHeight="10560" xr2:uid="{1D03AB2B-52FC-42D1-A358-4DB83B150D6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>RIVA128 to do:</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>Cursor (RAMDAC_CU)</t>
+  </si>
+  <si>
+    <t>Chroma Key</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Unify position/size structs</t>
+  </si>
+  <si>
+    <t>Code cleanup</t>
   </si>
 </sst>
 </file>
@@ -529,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7D5DA9-A0C6-4217-AFB0-C28D22984443}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -773,6 +785,26 @@
         <v>34</v>
       </c>
     </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>